<commit_message>
f/mmcdaniel-baroreceptors: More validation/documentation changes
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/DrugsValidation.xlsx
+++ b/share/doc/validation/Scenarios/DrugsValidation.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ProjectPrograms\BioGears\core\share\doc\validation\Scenarios\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="615" windowWidth="14880" windowHeight="3030" tabRatio="736" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="612" windowWidth="14880" windowHeight="3036" tabRatio="736" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="18" r:id="rId1"/>
@@ -18,7 +23,7 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$N$15</definedName>
   </definedNames>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -515,7 +520,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="25" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1376,6 +1381,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -1423,7 +1431,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1458,7 +1466,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1676,23 +1684,23 @@
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="1.85546875" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="1.85546875" style="46" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.140625" customWidth="1"/>
-    <col min="5" max="5" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8.7109375" style="11" customWidth="1"/>
-    <col min="7" max="7" width="27.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.7109375" customWidth="1"/>
-    <col min="9" max="9" width="26.5703125" style="46" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.7109375" customWidth="1"/>
-    <col min="12" max="12" width="9.140625" customWidth="1"/>
-    <col min="14" max="14" width="41.140625" customWidth="1"/>
+    <col min="1" max="1" width="1.88671875" style="36" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="1.88671875" style="46" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.109375" customWidth="1"/>
+    <col min="5" max="5" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.6640625" style="11" customWidth="1"/>
+    <col min="7" max="7" width="27.5546875" style="11" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" customWidth="1"/>
+    <col min="9" max="9" width="26.5546875" style="46" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.6640625" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" customWidth="1"/>
+    <col min="14" max="14" width="41.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
         <v>44</v>
       </c>
@@ -1727,7 +1735,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
         <v>44</v>
       </c>
@@ -1762,7 +1770,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
         <v>44</v>
       </c>
@@ -1801,7 +1809,7 @@
       <c r="N3" s="47"/>
       <c r="O3" s="47"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A4" s="48" t="s">
         <v>44</v>
       </c>
@@ -1840,7 +1848,7 @@
       <c r="N4" s="47"/>
       <c r="O4" s="47"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
         <v>44</v>
       </c>
@@ -1879,7 +1887,7 @@
       <c r="N5" s="47"/>
       <c r="O5" s="47"/>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
         <v>44</v>
       </c>
@@ -1918,7 +1926,7 @@
       <c r="N6" s="47"/>
       <c r="O6" s="47"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="48" t="s">
         <v>44</v>
       </c>
@@ -1957,7 +1965,7 @@
       <c r="N7" s="47"/>
       <c r="O7" s="47"/>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="54" t="s">
         <v>44</v>
       </c>
@@ -1996,7 +2004,7 @@
       <c r="N8" s="47"/>
       <c r="O8" s="47"/>
     </row>
-    <row r="9" spans="1:15" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A9" s="55" t="s">
         <v>44</v>
       </c>
@@ -2031,7 +2039,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="48" t="s">
         <v>44</v>
       </c>
@@ -2066,7 +2074,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="48" t="s">
         <v>44</v>
       </c>
@@ -2101,7 +2109,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A12" s="48" t="s">
         <v>44</v>
       </c>
@@ -2136,7 +2144,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="48" t="s">
         <v>44</v>
       </c>
@@ -2171,7 +2179,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="48" t="s">
         <v>44</v>
       </c>
@@ -2206,7 +2214,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:15" s="46" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" s="46" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="57" t="s">
         <v>44</v>
       </c>
@@ -2256,19 +2264,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.44140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.88671875" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="65.42578125" customWidth="1"/>
+    <col min="4" max="4" width="65.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
         <v>44</v>
       </c>
@@ -2279,7 +2287,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
         <v>44</v>
       </c>
@@ -2290,7 +2298,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
         <v>46</v>
       </c>
@@ -2301,7 +2309,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
         <v>49</v>
       </c>
@@ -2312,7 +2320,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
         <v>51</v>
       </c>
@@ -2335,36 +2343,36 @@
   </sheetPr>
   <dimension ref="A2:W16"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" style="39" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" style="39" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1" style="39" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" style="39" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" style="39" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1" style="39" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" style="39" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" style="39" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1" style="39" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" style="39" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.140625" style="39" customWidth="1"/>
-    <col min="17" max="17" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.28515625" style="39" customWidth="1"/>
-    <col min="19" max="19" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="27.28515625" style="39" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="18.5703125" style="39" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="8.140625" style="39" bestFit="1" customWidth="1"/>
-    <col min="24" max="16384" width="9.140625" style="39"/>
+    <col min="8" max="8" width="20.5546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" style="39" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.109375" style="39" customWidth="1"/>
+    <col min="17" max="17" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="24.33203125" style="39" customWidth="1"/>
+    <col min="19" max="19" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="27.33203125" style="39" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="18.5546875" style="39" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="8.109375" style="39" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9.109375" style="39"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:23" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
@@ -2438,7 +2446,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>44</v>
       </c>
@@ -2509,7 +2517,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:23" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>44</v>
       </c>
@@ -2580,7 +2588,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:23" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="P5" s="39" t="s">
         <v>40</v>
       </c>
@@ -2588,31 +2596,31 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:23" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D7" s="23"/>
       <c r="E7" s="23"/>
       <c r="F7" s="23"/>
       <c r="G7" s="23"/>
     </row>
-    <row r="8" spans="1:23" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D8" s="22"/>
       <c r="E8" s="22"/>
       <c r="F8" s="22"/>
       <c r="G8" s="22"/>
     </row>
-    <row r="9" spans="1:23" ht="13.9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D9" s="22"/>
       <c r="E9" s="22"/>
       <c r="F9" s="22"/>
       <c r="G9" s="22"/>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D10" s="23"/>
       <c r="E10" s="23"/>
       <c r="F10" s="23"/>
       <c r="G10" s="23"/>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B11" s="23"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -2620,29 +2628,29 @@
       <c r="F11" s="23"/>
       <c r="G11" s="23"/>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="B12" s="22"/>
       <c r="C12" s="22"/>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D13" s="23"/>
       <c r="E13" s="23"/>
       <c r="F13" s="23"/>
       <c r="G13" s="23"/>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D14" s="22"/>
       <c r="E14" s="22"/>
       <c r="F14" s="22"/>
       <c r="G14" s="22"/>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D15" s="23"/>
       <c r="E15" s="23"/>
       <c r="F15" s="23"/>
       <c r="G15" s="23"/>
     </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="D16" s="23"/>
       <c r="E16" s="23"/>
       <c r="F16" s="23"/>
@@ -2662,38 +2670,38 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <pane xSplit="2" topLeftCell="C1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F2" sqref="F2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="36.7109375" customWidth="1"/>
+    <col min="2" max="2" width="36.6640625" customWidth="1"/>
     <col min="3" max="3" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.7109375" customWidth="1"/>
+    <col min="4" max="4" width="36.6640625" customWidth="1"/>
     <col min="5" max="5" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="24.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5703125" style="74" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="36.7109375" customWidth="1"/>
-    <col min="11" max="11" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.7109375" customWidth="1"/>
-    <col min="13" max="13" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="36.7109375" customWidth="1"/>
-    <col min="15" max="15" width="31.5703125" style="36" customWidth="1"/>
-    <col min="16" max="16" width="36.7109375" customWidth="1"/>
-    <col min="17" max="17" width="29.7109375" style="36" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="36.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="36.6640625" customWidth="1"/>
+    <col min="11" max="11" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.6640625" customWidth="1"/>
+    <col min="13" max="13" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="36.6640625" customWidth="1"/>
+    <col min="15" max="15" width="31.5546875" style="36" customWidth="1"/>
+    <col min="16" max="16" width="36.6640625" customWidth="1"/>
+    <col min="17" max="17" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="36.6640625" customWidth="1"/>
     <col min="19" max="19" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="H1" s="74"/>
     </row>
-    <row r="2" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>44</v>
       </c>
@@ -2752,7 +2760,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
         <v>44</v>
       </c>
@@ -2811,7 +2819,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:19" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
         <v>44</v>
       </c>
@@ -2870,7 +2878,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
         <v>44</v>
       </c>
@@ -2929,7 +2937,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:19" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
         <v>44</v>
       </c>
@@ -2988,7 +2996,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:19" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
         <v>44</v>
       </c>
@@ -3047,7 +3055,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
         <v>44</v>
       </c>
@@ -3106,7 +3114,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="s">
         <v>44</v>
       </c>
@@ -3165,7 +3173,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="42" t="s">
         <v>44</v>
       </c>
@@ -3224,7 +3232,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
         <v>44</v>
       </c>
@@ -3283,7 +3291,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="s">
         <v>44</v>
       </c>
@@ -3342,7 +3350,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="42" t="s">
         <v>44</v>
       </c>
@@ -3401,7 +3409,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="14" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="42" t="s">
         <v>44</v>
       </c>
@@ -3474,27 +3482,27 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5546875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.44140625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="20.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="25.28515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="27.28515625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="25.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="20.5546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="25.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" s="39"/>
       <c r="B1" s="39"/>
       <c r="C1" s="39"/>
@@ -3512,7 +3520,7 @@
       <c r="P1" s="39"/>
       <c r="Q1" s="39"/>
     </row>
-    <row r="2" spans="1:17" ht="26.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
         <v>44</v>
       </c>
@@ -3565,7 +3573,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
         <v>44</v>
       </c>
@@ -3618,7 +3626,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="4" spans="1:17" ht="43.15" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
         <v>44</v>
       </c>
@@ -3671,7 +3679,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5" s="39"/>
       <c r="B5" s="39"/>
       <c r="C5" s="39"/>
@@ -3690,7 +3698,7 @@
       <c r="P5" s="39"/>
       <c r="Q5" s="39"/>
     </row>
-    <row r="6" spans="1:17" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6" s="39"/>
       <c r="B6" s="39"/>
       <c r="C6" s="39"/>
@@ -3723,31 +3731,31 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="16.85546875" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="4" width="21.28515625" customWidth="1"/>
-    <col min="5" max="5" width="2.42578125" customWidth="1"/>
-    <col min="6" max="6" width="27.28515625" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
-    <col min="9" max="9" width="29.140625" customWidth="1"/>
-    <col min="10" max="10" width="25.85546875" customWidth="1"/>
-    <col min="11" max="11" width="32.7109375" customWidth="1"/>
-    <col min="12" max="12" width="18.5703125" customWidth="1"/>
-    <col min="13" max="13" width="31.7109375" customWidth="1"/>
-    <col min="14" max="14" width="25.85546875" customWidth="1"/>
-    <col min="15" max="15" width="31.140625" customWidth="1"/>
-    <col min="16" max="16" width="21.140625" customWidth="1"/>
-    <col min="17" max="17" width="29.42578125" customWidth="1"/>
-    <col min="18" max="18" width="22.7109375" customWidth="1"/>
+    <col min="1" max="1" width="3.6640625" customWidth="1"/>
+    <col min="2" max="2" width="16.88671875" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="21.33203125" customWidth="1"/>
+    <col min="5" max="5" width="2.44140625" customWidth="1"/>
+    <col min="6" max="6" width="27.33203125" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="25.6640625" customWidth="1"/>
+    <col min="9" max="9" width="29.109375" customWidth="1"/>
+    <col min="10" max="10" width="25.88671875" customWidth="1"/>
+    <col min="11" max="11" width="32.6640625" customWidth="1"/>
+    <col min="12" max="12" width="18.5546875" customWidth="1"/>
+    <col min="13" max="13" width="31.6640625" customWidth="1"/>
+    <col min="14" max="14" width="25.88671875" customWidth="1"/>
+    <col min="15" max="15" width="31.109375" customWidth="1"/>
+    <col min="16" max="16" width="21.109375" customWidth="1"/>
+    <col min="17" max="17" width="29.44140625" customWidth="1"/>
+    <col min="18" max="18" width="22.6640625" customWidth="1"/>
     <col min="19" max="19" width="31" customWidth="1"/>
-    <col min="20" max="20" width="23.28515625" customWidth="1"/>
+    <col min="20" max="20" width="23.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:21" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>44</v>
       </c>
@@ -3812,7 +3820,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>44</v>
       </c>
@@ -3942,7 +3950,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="5" spans="1:21" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
       <c r="B5" s="76"/>
       <c r="C5" s="1"/>
@@ -3952,7 +3960,7 @@
       <c r="G5" s="1"/>
       <c r="H5" s="76"/>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
       <c r="B6" s="76"/>
       <c r="C6" s="1"/>
@@ -3962,7 +3970,7 @@
       <c r="G6" s="1"/>
       <c r="H6" s="76"/>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
       <c r="C7" s="1"/>
       <c r="E7" s="1"/>
@@ -3981,30 +3989,30 @@
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="3" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="2.7109375" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
-    <col min="5" max="5" width="2.28515625" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" customWidth="1"/>
-    <col min="7" max="7" width="2.7109375" customWidth="1"/>
-    <col min="8" max="8" width="24.28515625" customWidth="1"/>
-    <col min="9" max="9" width="17.7109375" customWidth="1"/>
-    <col min="10" max="10" width="22.85546875" customWidth="1"/>
-    <col min="11" max="11" width="18.28515625" customWidth="1"/>
-    <col min="12" max="12" width="20.140625" customWidth="1"/>
-    <col min="13" max="13" width="13.7109375" customWidth="1"/>
-    <col min="14" max="14" width="20.5703125" customWidth="1"/>
-    <col min="15" max="15" width="13.42578125" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" customWidth="1"/>
+    <col min="2" max="2" width="28.88671875" customWidth="1"/>
+    <col min="3" max="3" width="2.6640625" customWidth="1"/>
+    <col min="4" max="4" width="17.88671875" customWidth="1"/>
+    <col min="5" max="5" width="2.33203125" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" customWidth="1"/>
+    <col min="7" max="7" width="2.6640625" customWidth="1"/>
+    <col min="8" max="8" width="24.33203125" customWidth="1"/>
+    <col min="9" max="9" width="17.6640625" customWidth="1"/>
+    <col min="10" max="10" width="22.88671875" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" customWidth="1"/>
+    <col min="12" max="12" width="20.109375" customWidth="1"/>
+    <col min="13" max="13" width="13.6640625" customWidth="1"/>
+    <col min="14" max="14" width="20.5546875" customWidth="1"/>
+    <col min="15" max="15" width="13.44140625" customWidth="1"/>
+    <col min="16" max="16" width="19.88671875" customWidth="1"/>
     <col min="17" max="17" width="13" customWidth="1"/>
-    <col min="18" max="18" width="21.28515625" customWidth="1"/>
-    <col min="20" max="20" width="19.42578125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="21.33203125" customWidth="1"/>
+    <col min="20" max="20" width="19.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
         <v>44</v>
       </c>
@@ -4064,7 +4072,7 @@
       </c>
       <c r="T1" s="53"/>
     </row>
-    <row r="2" spans="1:20" ht="14.45" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
         <v>44</v>
       </c>

</xml_diff>

<commit_message>
f/mmcdaniel-baroreceptors: Update drug methodology, fix broken ref
</commit_message>
<xml_diff>
--- a/share/doc/validation/Scenarios/DrugsValidation.xlsx
+++ b/share/doc/validation/Scenarios/DrugsValidation.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="612" windowWidth="14880" windowHeight="3036" tabRatio="736" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="240" yWindow="612" windowWidth="14880" windowHeight="3036" tabRatio="736"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="18" r:id="rId1"/>
@@ -21,14 +21,14 @@
     <sheet name="Morphine" sheetId="28" r:id="rId7"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$N$15</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Summary!$B$1:$N$20</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="622" uniqueCount="154">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="166">
   <si>
     <t>Event</t>
   </si>
@@ -121,9 +121,6 @@
   </si>
   <si>
     <t>Morphine</t>
-  </si>
-  <si>
-    <t>Administer 42 mg injection of Morphine</t>
   </si>
   <si>
     <t>Administer 52 mg injection of Rocuronium</t>
@@ -515,6 +512,45 @@
   </si>
   <si>
     <t>Action Occurrence Time (s)</t>
+  </si>
+  <si>
+    <t>Ramp dose of vasopressin from 0.04 to 0.18 to 0.25 ug</t>
+  </si>
+  <si>
+    <t>Vasopressin</t>
+  </si>
+  <si>
+    <t>Desflurane</t>
+  </si>
+  <si>
+    <t>6% Desflurane breathed in through mask</t>
+  </si>
+  <si>
+    <t>Morphine Overdose</t>
+  </si>
+  <si>
+    <t>Administer 2.75 mg/min IV Morphine for 4 minutes</t>
+  </si>
+  <si>
+    <t>Administer 8.2 mg/min IV Morphine for 24 minutes</t>
+  </si>
+  <si>
+    <t>Furosemide</t>
+  </si>
+  <si>
+    <t>Administer 40 mg of Furosemide</t>
+  </si>
+  <si>
+    <t>Sarin</t>
+  </si>
+  <si>
+    <t>Exposure to 5 concentrations in the environment</t>
+  </si>
+  <si>
+    <t>Tranexamic Acid</t>
+  </si>
+  <si>
+    <t>Administer 200 mg of TXA</t>
   </si>
 </sst>
 </file>
@@ -1117,7 +1153,7 @@
       <alignment wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="80">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1304,9 +1340,6 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1678,10 +1711,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:O15"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1702,146 +1735,146 @@
   <sheetData>
     <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="49" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="C1" s="56" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="7" t="s">
         <v>15</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="45" t="s">
+        <v>76</v>
+      </c>
+      <c r="G1" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="H1" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="G1" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="H1" s="44" t="s">
+      <c r="I1" s="50" t="s">
+        <v>43</v>
+      </c>
+      <c r="J1" s="43" t="s">
         <v>78</v>
       </c>
-      <c r="I1" s="50" t="s">
-        <v>44</v>
-      </c>
-      <c r="J1" s="43" t="s">
-        <v>79</v>
-      </c>
       <c r="K1" s="52" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A2" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E2" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I2" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K2" s="66" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C3" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="E3" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F3" s="10">
         <v>5</v>
       </c>
       <c r="G3" s="67" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H3" s="8">
         <v>0</v>
       </c>
       <c r="I3" s="70" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J3" s="9">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L3" s="47"/>
       <c r="M3" s="47"/>
       <c r="N3" s="47"/>
       <c r="O3" s="47"/>
     </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A4" s="48" t="s">
-        <v>44</v>
+    <row r="4" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="66" t="s">
+        <v>43</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C4" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>24</v>
+        <v>155</v>
+      </c>
+      <c r="C4" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="42" t="s">
+        <v>156</v>
       </c>
       <c r="E4" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F4" s="10">
         <v>4</v>
       </c>
-      <c r="G4" s="67" t="s">
+      <c r="G4" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H4" s="8">
+        <v>2</v>
+      </c>
+      <c r="I4" s="72" t="s">
         <v>81</v>
-      </c>
-      <c r="H4" s="8">
-        <v>1</v>
-      </c>
-      <c r="I4" s="70" t="s">
-        <v>82</v>
       </c>
       <c r="J4" s="9">
         <v>0</v>
       </c>
       <c r="K4" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L4" s="47"/>
       <c r="M4" s="47"/>
@@ -1850,37 +1883,37 @@
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C5" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="E5" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F5" s="10">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G5" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H5" s="8">
+        <v>1</v>
+      </c>
+      <c r="I5" s="70" t="s">
         <v>81</v>
-      </c>
-      <c r="H5" s="8">
-        <v>0</v>
-      </c>
-      <c r="I5" s="70" t="s">
-        <v>82</v>
       </c>
       <c r="J5" s="9">
         <v>0</v>
       </c>
       <c r="K5" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L5" s="47"/>
       <c r="M5" s="47"/>
@@ -1889,76 +1922,76 @@
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C6" s="55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="E6" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F6" s="10">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G6" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H6" s="8">
+        <v>0</v>
+      </c>
+      <c r="I6" s="70" t="s">
         <v>81</v>
-      </c>
-      <c r="H6" s="8">
-        <v>1</v>
-      </c>
-      <c r="I6" s="70" t="s">
-        <v>82</v>
       </c>
       <c r="J6" s="9">
         <v>0</v>
       </c>
       <c r="K6" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L6" s="47"/>
       <c r="M6" s="47"/>
       <c r="N6" s="47"/>
       <c r="O6" s="47"/>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A7" s="48" t="s">
-        <v>44</v>
+    <row r="7" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="66" t="s">
+        <v>43</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C7" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="5" t="s">
-        <v>28</v>
+        <v>160</v>
+      </c>
+      <c r="C7" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="42" t="s">
+        <v>161</v>
       </c>
       <c r="E7" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F7" s="10">
-        <v>5</v>
-      </c>
-      <c r="G7" s="68" t="s">
+        <v>3</v>
+      </c>
+      <c r="G7" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H7" s="8">
+        <v>1</v>
+      </c>
+      <c r="I7" s="72" t="s">
         <v>81</v>
-      </c>
-      <c r="H7" s="8">
-        <v>0</v>
-      </c>
-      <c r="I7" s="71" t="s">
-        <v>82</v>
       </c>
       <c r="J7" s="9">
         <v>0</v>
       </c>
       <c r="K7" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L7" s="47"/>
       <c r="M7" s="47"/>
@@ -1966,288 +1999,510 @@
       <c r="O7" s="47"/>
     </row>
     <row r="8" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A8" s="54" t="s">
-        <v>44</v>
+      <c r="A8" s="48" t="s">
+        <v>43</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="C8" s="54" t="s">
-        <v>44</v>
+        <v>18</v>
+      </c>
+      <c r="C8" s="55" t="s">
+        <v>43</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="E8" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" s="10">
-        <v>5</v>
-      </c>
-      <c r="G8" s="68" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="67" t="s">
+        <v>80</v>
+      </c>
+      <c r="H8" s="8">
+        <v>1</v>
+      </c>
+      <c r="I8" s="70" t="s">
         <v>81</v>
-      </c>
-      <c r="H8" s="8">
-        <v>0</v>
-      </c>
-      <c r="I8" s="71" t="s">
-        <v>82</v>
       </c>
       <c r="J8" s="9">
         <v>0</v>
       </c>
       <c r="K8" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L8" s="47"/>
       <c r="M8" s="47"/>
       <c r="N8" s="47"/>
       <c r="O8" s="47"/>
     </row>
-    <row r="9" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A9" s="55" t="s">
-        <v>44</v>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A9" s="48" t="s">
+        <v>43</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C9" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>83</v>
+        <v>43</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>28</v>
       </c>
       <c r="E9" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F9" s="10">
         <v>5</v>
       </c>
       <c r="G9" s="68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H9" s="8">
         <v>0</v>
       </c>
       <c r="I9" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J9" s="9">
         <v>0</v>
       </c>
       <c r="K9" s="51" t="s">
-        <v>48</v>
-      </c>
+        <v>47</v>
+      </c>
+      <c r="L9" s="47"/>
+      <c r="M9" s="47"/>
+      <c r="N9" s="47"/>
+      <c r="O9" s="47"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A10" s="48" t="s">
-        <v>44</v>
+      <c r="A10" s="54" t="s">
+        <v>43</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="C10" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>41</v>
+        <v>29</v>
+      </c>
+      <c r="C10" s="54" t="s">
+        <v>43</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>158</v>
       </c>
       <c r="E10" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F10" s="10">
         <v>5</v>
       </c>
       <c r="G10" s="68" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H10" s="8">
         <v>0</v>
       </c>
       <c r="I10" s="71" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J10" s="9">
         <v>0</v>
       </c>
       <c r="K10" s="51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A11" s="48" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="L10" s="47"/>
+      <c r="M10" s="47"/>
+      <c r="N10" s="47"/>
+      <c r="O10" s="47"/>
+    </row>
+    <row r="11" spans="1:15" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="65" t="s">
+        <v>43</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="C11" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>42</v>
+        <v>157</v>
+      </c>
+      <c r="C11" s="65" t="s">
+        <v>43</v>
+      </c>
+      <c r="D11" s="42" t="s">
+        <v>159</v>
       </c>
       <c r="E11" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F11" s="10">
-        <v>5</v>
-      </c>
-      <c r="G11" s="69" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H11" s="8">
+        <v>2</v>
+      </c>
+      <c r="I11" s="72" t="s">
         <v>81</v>
-      </c>
-      <c r="H11" s="8">
-        <v>0</v>
-      </c>
-      <c r="I11" s="72" t="s">
-        <v>82</v>
       </c>
       <c r="J11" s="9">
         <v>0</v>
       </c>
       <c r="K11" s="51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="12" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A12" s="48" t="s">
-        <v>44</v>
+        <v>47</v>
+      </c>
+      <c r="L11" s="47"/>
+      <c r="M11" s="47"/>
+      <c r="N11" s="47"/>
+      <c r="O11" s="47"/>
+    </row>
+    <row r="12" spans="1:15" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="A12" s="55" t="s">
+        <v>43</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C12" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D12" s="5" t="s">
-        <v>32</v>
+        <v>43</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>82</v>
       </c>
       <c r="E12" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F12" s="10">
-        <v>4</v>
-      </c>
-      <c r="G12" s="69" t="s">
+        <v>5</v>
+      </c>
+      <c r="G12" s="68" t="s">
+        <v>80</v>
+      </c>
+      <c r="H12" s="8">
+        <v>0</v>
+      </c>
+      <c r="I12" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="H12" s="16">
+      <c r="J12" s="9">
         <v>0</v>
       </c>
-      <c r="I12" s="72" t="s">
-        <v>82</v>
-      </c>
-      <c r="J12" s="17">
-        <v>1</v>
-      </c>
       <c r="K12" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>22</v>
+        <v>35</v>
       </c>
       <c r="C13" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D13" s="5" t="s">
-        <v>31</v>
+        <v>43</v>
+      </c>
+      <c r="D13" s="1" t="s">
+        <v>40</v>
       </c>
       <c r="E13" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F13" s="10">
-        <v>2</v>
-      </c>
-      <c r="G13" s="69" t="s">
-        <v>81</v>
+        <v>5</v>
+      </c>
+      <c r="G13" s="68" t="s">
+        <v>80</v>
       </c>
       <c r="H13" s="8">
         <v>0</v>
       </c>
-      <c r="I13" s="72" t="s">
-        <v>82</v>
+      <c r="I13" s="71" t="s">
+        <v>81</v>
       </c>
       <c r="J13" s="9">
-        <v>3</v>
+        <v>0</v>
       </c>
       <c r="K13" s="51" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="48" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="C14" s="55" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>33</v>
+        <v>43</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>41</v>
       </c>
       <c r="E14" s="65" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F14" s="10">
         <v>5</v>
       </c>
       <c r="G14" s="69" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="H14" s="8">
         <v>0</v>
       </c>
       <c r="I14" s="72" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="J14" s="9">
         <v>0</v>
       </c>
       <c r="K14" s="51" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" s="46" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="B15" s="58"/>
-      <c r="C15" s="57" t="s">
-        <v>44</v>
-      </c>
-      <c r="D15" s="59" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A15" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E15" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F15" s="10">
+        <v>4</v>
+      </c>
+      <c r="G15" s="69" t="s">
         <v>80</v>
       </c>
-      <c r="E15" s="57" t="s">
-        <v>46</v>
-      </c>
-      <c r="F15" s="60">
-        <f>SUM(F3:F14)</f>
-        <v>54</v>
-      </c>
-      <c r="G15" s="61" t="s">
+      <c r="H15" s="16">
+        <v>0</v>
+      </c>
+      <c r="I15" s="72" t="s">
         <v>81</v>
       </c>
-      <c r="H15" s="62">
-        <f>SUM(H3:H14)</f>
+      <c r="J15" s="17">
+        <v>0</v>
+      </c>
+      <c r="K15" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+      <c r="A16" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C16" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D16" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="E16" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F16" s="10">
         <v>2</v>
       </c>
-      <c r="I15" s="61" t="s">
-        <v>82</v>
-      </c>
-      <c r="J15" s="63">
-        <f>SUM(J3:J14)</f>
-        <v>5</v>
-      </c>
-      <c r="K15" s="64" t="s">
-        <v>48</v>
+      <c r="G16" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="H16" s="8">
+        <v>0</v>
+      </c>
+      <c r="I16" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J16" s="9">
+        <v>0</v>
+      </c>
+      <c r="K16" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="C17" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D17" s="42" t="s">
+        <v>163</v>
+      </c>
+      <c r="E17" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F17" s="10">
+        <v>21</v>
+      </c>
+      <c r="G17" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H17" s="8">
+        <v>4</v>
+      </c>
+      <c r="I17" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J17" s="9">
+        <v>0</v>
+      </c>
+      <c r="K17" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A18" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C18" s="55" t="s">
+        <v>43</v>
+      </c>
+      <c r="D18" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F18" s="10">
+        <v>3</v>
+      </c>
+      <c r="G18" s="69" t="s">
+        <v>80</v>
+      </c>
+      <c r="H18" s="8">
+        <v>2</v>
+      </c>
+      <c r="I18" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J18" s="9">
+        <v>0</v>
+      </c>
+      <c r="K18" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" s="53" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="C19" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D19" s="42" t="s">
+        <v>165</v>
+      </c>
+      <c r="E19" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F19" s="10">
+        <v>8</v>
+      </c>
+      <c r="G19" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H19" s="8">
+        <v>0</v>
+      </c>
+      <c r="I19" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J19" s="9">
+        <v>0</v>
+      </c>
+      <c r="K19" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" s="46" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C20" s="66" t="s">
+        <v>43</v>
+      </c>
+      <c r="D20" s="42" t="s">
+        <v>153</v>
+      </c>
+      <c r="E20" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="F20" s="10">
+        <v>3</v>
+      </c>
+      <c r="G20" s="72" t="s">
+        <v>80</v>
+      </c>
+      <c r="H20" s="8">
+        <v>2</v>
+      </c>
+      <c r="I20" s="72" t="s">
+        <v>81</v>
+      </c>
+      <c r="J20" s="9">
+        <v>0</v>
+      </c>
+      <c r="K20" s="51" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="A21" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="58"/>
+      <c r="C21" s="57" t="s">
+        <v>43</v>
+      </c>
+      <c r="D21" s="59" t="s">
+        <v>79</v>
+      </c>
+      <c r="E21" s="57" t="s">
+        <v>45</v>
+      </c>
+      <c r="F21" s="60">
+        <f>SUM(F3:F20)</f>
+        <v>94</v>
+      </c>
+      <c r="G21" s="61" t="s">
+        <v>80</v>
+      </c>
+      <c r="H21" s="62">
+        <f>SUM(H3:H20)</f>
+        <v>15</v>
+      </c>
+      <c r="I21" s="61" t="s">
+        <v>81</v>
+      </c>
+      <c r="J21" s="63">
+        <f>SUM(J3:J20)</f>
+        <v>0</v>
+      </c>
+      <c r="K21" s="64" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2278,57 +2533,57 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="33" t="s">
         <v>25</v>
       </c>
       <c r="C1" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C2" s="31" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3" s="31" t="s">
+        <v>45</v>
+      </c>
+      <c r="B3" s="29" t="s">
         <v>46</v>
       </c>
-      <c r="B3" s="29" t="s">
+      <c r="C3" s="31" t="s">
         <v>47</v>
-      </c>
-      <c r="C3" s="31" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4" s="31" t="s">
+        <v>48</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>49</v>
       </c>
-      <c r="B4" s="34" t="s">
-        <v>50</v>
-      </c>
       <c r="C4" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" s="31" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="30" t="s">
         <v>51</v>
       </c>
-      <c r="B5" s="30" t="s">
-        <v>52</v>
-      </c>
       <c r="C5" s="31" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -2377,223 +2632,223 @@
   <sheetData>
     <row r="2" spans="1:23" ht="43.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="28" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="27" t="s">
         <v>4</v>
       </c>
       <c r="K2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="19" t="s">
         <v>5</v>
       </c>
       <c r="M2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N2" s="19" t="s">
         <v>6</v>
       </c>
       <c r="O2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P2" s="19" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="Q2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R2" s="19" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="S2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T2" s="19" t="s">
         <v>2</v>
       </c>
       <c r="U2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V2" s="19" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="W2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="U3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="V3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="W3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:23" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="41">
         <v>30</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="35">
         <v>200</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="25" t="s">
+        <v>52</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="K4" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="12" t="s">
+      <c r="M4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>53</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="M4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="25" t="s">
+      <c r="Q4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="O4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="Q4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="20" t="s">
-        <v>55</v>
-      </c>
       <c r="S4" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="T4" s="26" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="U4" s="40" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="V4" s="20" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="W4" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="P5" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="R5" s="39" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.3">
@@ -2670,9 +2925,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:S14"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <pane xSplit="2" topLeftCell="J1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="J6" sqref="J6"/>
+      <selection pane="topRight" activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2684,7 +2939,7 @@
     <col min="5" max="5" width="2" style="36" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="24.33203125" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="2" style="36" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.5546875" style="74" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="23.5546875" style="73" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="36.6640625" customWidth="1"/>
     <col min="11" max="11" width="29.6640625" style="36" bestFit="1" customWidth="1"/>
@@ -2699,773 +2954,773 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="H1" s="74"/>
+      <c r="H1" s="73"/>
     </row>
     <row r="2" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="18" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="18" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="18" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="18" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="K2" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="K2" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="4" t="s">
+      <c r="M2" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>62</v>
       </c>
-      <c r="M2" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="4" t="s">
         <v>63</v>
       </c>
-      <c r="O2" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="4" t="s">
-        <v>64</v>
-      </c>
       <c r="Q2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R2" s="4" t="s">
         <v>2</v>
       </c>
       <c r="S2" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:19" s="36" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R3" s="24" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="S3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>13</v>
       </c>
       <c r="C4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1">
         <v>30</v>
       </c>
       <c r="G4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3">
         <v>30</v>
       </c>
       <c r="I4" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="K4" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L4" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="M4" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="15" t="s">
+        <v>56</v>
+      </c>
+      <c r="O4" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="M4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="15" t="s">
-        <v>57</v>
-      </c>
-      <c r="O4" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>58</v>
-      </c>
       <c r="Q4" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R4" s="14" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S4" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A5" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C5" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E5" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" s="1">
         <v>30</v>
       </c>
       <c r="G5" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H5" s="3">
         <v>600</v>
       </c>
       <c r="I5" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J5" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="K5" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L5" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="M5" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N5" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="O5" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P5" s="15" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="Q5" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R5" s="15" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="S5" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="6" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A6" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>10</v>
       </c>
       <c r="C6" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D6" s="42" t="s">
         <v>7</v>
       </c>
       <c r="E6" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" s="42">
         <v>30</v>
       </c>
       <c r="G6" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H6" s="2">
         <v>300</v>
       </c>
       <c r="I6" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="K6" s="42" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="L6" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="M6" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N6" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="O6" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P6" s="15" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="Q6" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R6" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="S6" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="7" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A7" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C7" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E7" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F7" s="1">
         <v>30</v>
       </c>
       <c r="G7" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H7" s="3">
         <v>70</v>
       </c>
       <c r="I7" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J7" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="K7" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L7" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="M7" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N7" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="O7" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P7" s="15" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="Q7" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R7" s="13" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="S7" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="8" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A8" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="C8" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D8" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="C8" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>127</v>
-      </c>
       <c r="E8" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G8" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H8" s="3">
         <v>5000</v>
       </c>
       <c r="I8" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J8" s="13" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="K8" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L8" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="M8" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N8" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="O8" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P8" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="Q8" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R8" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="S8" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="9" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A9" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="C9" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D9" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C9" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D9" s="1" t="s">
+      <c r="E9" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="E9" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="G9" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>139</v>
-      </c>
       <c r="I9" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J9" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="L9" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="M9" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="N9" s="15" t="s">
+        <v>143</v>
+      </c>
+      <c r="O9" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="P9" s="15" t="s">
         <v>144</v>
       </c>
-      <c r="K9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="L9" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="M9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="N9" s="15" t="s">
-        <v>144</v>
-      </c>
-      <c r="O9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="P9" s="15" t="s">
+      <c r="Q9" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="R9" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="Q9" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>146</v>
-      </c>
       <c r="S9" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="10" spans="1:19" x14ac:dyDescent="0.3">
       <c r="A10" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D10" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E10" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F10" s="1">
         <v>30</v>
       </c>
       <c r="G10" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H10" s="3">
         <v>100</v>
       </c>
       <c r="I10" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="K10" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="M10" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="O10" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Q10" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R10" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="S10" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="11" spans="1:19" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A11" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C11" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>11</v>
       </c>
       <c r="E11" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F11" s="1">
         <v>30</v>
       </c>
       <c r="G11" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H11" s="3">
         <v>70</v>
       </c>
       <c r="I11" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="J11" s="73" t="s">
-        <v>68</v>
+        <v>45</v>
+      </c>
+      <c r="J11" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="K11" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="M11" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N11" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="O11" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P11" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="Q11" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R11" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S11" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E12" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F12" s="1">
         <v>30</v>
       </c>
       <c r="G12" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H12" s="3">
         <v>100</v>
       </c>
       <c r="I12" s="42" t="s">
-        <v>51</v>
-      </c>
-      <c r="J12" s="73" t="s">
-        <v>69</v>
+        <v>45</v>
+      </c>
+      <c r="J12" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="K12" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L12" s="15" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="M12" s="42" t="s">
-        <v>82</v>
-      </c>
-      <c r="N12" s="73" t="s">
-        <v>69</v>
+        <v>55</v>
+      </c>
+      <c r="N12" s="15" t="s">
+        <v>68</v>
       </c>
       <c r="O12" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P12" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q12" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R12" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S12" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="13" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A13" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B13" s="42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C13" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D13" s="42" t="s">
         <v>7</v>
       </c>
       <c r="E13" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F13" s="42">
         <v>30</v>
       </c>
       <c r="G13" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H13" s="2">
         <v>70</v>
       </c>
       <c r="I13" s="42" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="J13" s="12" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="K13" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>70</v>
+        <v>55</v>
+      </c>
+      <c r="L13" s="15" t="s">
+        <v>69</v>
       </c>
       <c r="M13" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="N13" s="15" t="s">
-        <v>70</v>
+        <v>80</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>69</v>
       </c>
       <c r="O13" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="P13" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="Q13" s="42" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R13" s="13" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="S13" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:19" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A14" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B14" s="42" t="s">
+        <v>146</v>
+      </c>
+      <c r="C14" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="D14" s="42" t="s">
         <v>147</v>
       </c>
-      <c r="C14" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="D14" s="42" t="s">
+      <c r="E14" s="42" t="s">
+        <v>43</v>
+      </c>
+      <c r="F14" s="42" t="s">
         <v>148</v>
       </c>
-      <c r="E14" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="F14" s="42" t="s">
-        <v>149</v>
-      </c>
       <c r="G14" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H14" s="2">
         <v>2430</v>
       </c>
       <c r="I14" s="42" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J14" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="K14" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="L14" s="12" t="s">
         <v>150</v>
       </c>
-      <c r="K14" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="L14" s="12" t="s">
+      <c r="M14" s="42" t="s">
+        <v>80</v>
+      </c>
+      <c r="N14" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="O14" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="P14" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="M14" s="42" t="s">
-        <v>81</v>
-      </c>
-      <c r="N14" s="12" t="s">
+      <c r="Q14" s="42" t="s">
+        <v>55</v>
+      </c>
+      <c r="R14" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="O14" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="P14" s="15" t="s">
-        <v>152</v>
-      </c>
-      <c r="Q14" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="R14" s="15" t="s">
-        <v>152</v>
-      </c>
       <c r="S14" s="42" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -3522,161 +3777,161 @@
     </row>
     <row r="2" spans="1:17" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="38" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="38" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="28" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="28" t="s">
+        <v>89</v>
+      </c>
+      <c r="I2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="J2" s="27" t="s">
         <v>90</v>
       </c>
-      <c r="I2" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="27" t="s">
+      <c r="K2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="L2" s="19" t="s">
         <v>91</v>
       </c>
-      <c r="K2" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="19" t="s">
+      <c r="M2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="19" t="s">
         <v>92</v>
       </c>
-      <c r="M2" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="19" t="s">
+      <c r="O2" s="21" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="19" t="s">
         <v>93</v>
       </c>
-      <c r="O2" s="21" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="19" t="s">
-        <v>94</v>
-      </c>
       <c r="Q2" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="E3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="I3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="K3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="M3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="N3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="O3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="P3" s="37" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q3" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:17" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="41" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="41">
         <v>30</v>
       </c>
       <c r="G4" s="21" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="35">
         <v>450</v>
       </c>
       <c r="I4" s="40" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="K4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="74" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="40" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="25" t="s">
+        <v>87</v>
+      </c>
+      <c r="O4" s="40" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="K4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="75" t="s">
-        <v>88</v>
-      </c>
-      <c r="M4" s="40" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="25" t="s">
-        <v>88</v>
-      </c>
-      <c r="O4" s="40" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" s="12" t="s">
-        <v>89</v>
-      </c>
       <c r="Q4" s="40" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:17" x14ac:dyDescent="0.3">
@@ -3728,7 +3983,7 @@
   <dimension ref="A2:U7"/>
   <sheetViews>
     <sheetView zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="L4" sqref="L4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3757,218 +4012,218 @@
   <sheetData>
     <row r="2" spans="1:21" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B2" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F2" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H2" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J2" s="4" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L2" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N2" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="4" t="s">
+      <c r="O2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="R2" s="4" t="s">
         <v>101</v>
       </c>
-      <c r="O2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="4" t="s">
+      <c r="S2" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="4" t="s">
         <v>98</v>
       </c>
-      <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="4" t="s">
-        <v>102</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="4" t="s">
-        <v>99</v>
-      </c>
       <c r="U2" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="B3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="D3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="H3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="J3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="L3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="N3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="O3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="P3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="Q3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="R3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T3" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="T3" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="4" spans="1:21" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F4" s="1">
         <v>80</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3">
         <v>1000</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="J4" s="77" t="s">
+        <v>45</v>
+      </c>
+      <c r="J4" s="76" t="s">
+        <v>105</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="L4" s="77" t="s">
         <v>106</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="L4" s="78" t="s">
+      <c r="M4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="N4" s="76" t="s">
         <v>107</v>
       </c>
-      <c r="M4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="N4" s="77" t="s">
+      <c r="O4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="P4" s="77" t="s">
         <v>108</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="P4" s="78" t="s">
-        <v>109</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="R4" s="77" t="s">
+        <v>55</v>
+      </c>
+      <c r="R4" s="76" t="s">
+        <v>103</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="T4" s="76" t="s">
         <v>104</v>
       </c>
-      <c r="S4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="T4" s="77" t="s">
-        <v>105</v>
-      </c>
       <c r="U4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A5" s="1"/>
-      <c r="B5" s="76"/>
+      <c r="B5" s="75"/>
       <c r="C5" s="1"/>
-      <c r="D5" s="76"/>
+      <c r="D5" s="75"/>
       <c r="E5" s="1"/>
-      <c r="F5" s="76"/>
+      <c r="F5" s="75"/>
       <c r="G5" s="1"/>
-      <c r="H5" s="76"/>
+      <c r="H5" s="75"/>
     </row>
     <row r="6" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A6" s="1"/>
-      <c r="B6" s="76"/>
+      <c r="B6" s="75"/>
       <c r="C6" s="1"/>
-      <c r="D6" s="76"/>
+      <c r="D6" s="75"/>
       <c r="E6" s="1"/>
-      <c r="F6" s="76"/>
+      <c r="F6" s="75"/>
       <c r="G6" s="1"/>
-      <c r="H6" s="76"/>
+      <c r="H6" s="75"/>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
@@ -3985,7 +4240,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T4"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
@@ -4014,241 +4269,241 @@
   <sheetData>
     <row r="1" spans="1:20" ht="43.2" x14ac:dyDescent="0.3">
       <c r="A1" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F1" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H1" s="4" t="s">
         <v>3</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J1" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="L1" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="N1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N1" s="4" t="s">
+      <c r="O1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>113</v>
-      </c>
       <c r="Q1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="S1" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="T1" s="53"/>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" s="42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="B2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="D2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="F2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="H2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="I2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="J2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="J2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="K2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="L2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="L2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="M2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="N2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="N2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="O2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="P2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="R2" s="76" t="s">
-        <v>45</v>
+        <v>43</v>
+      </c>
+      <c r="R2" s="75" t="s">
+        <v>44</v>
       </c>
       <c r="S2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T2" s="79"/>
+        <v>43</v>
+      </c>
+      <c r="T2" s="78"/>
     </row>
     <row r="3" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A3" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D3" s="1" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>120</v>
-      </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H3" s="3">
         <v>5000</v>
       </c>
       <c r="I3" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J3" s="15" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="M3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="N3" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P3" s="13" t="s">
         <v>114</v>
       </c>
-      <c r="O3" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P3" s="13" t="s">
-        <v>115</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="R3" s="15" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T3" s="53"/>
     </row>
     <row r="4" spans="1:20" ht="57.6" x14ac:dyDescent="0.3">
       <c r="A4" s="42" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="D4" s="1" t="s">
         <v>121</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D4" s="1" t="s">
+      <c r="E4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="E4" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>123</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="H4" s="3">
         <v>7200</v>
       </c>
       <c r="I4" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="J4" s="15" t="s">
+        <v>115</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="L4" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="12" t="s">
         <v>116</v>
       </c>
-      <c r="K4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="L4" s="15" t="s">
-        <v>130</v>
-      </c>
-      <c r="M4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="N4" s="12" t="s">
+      <c r="O4" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="P4" s="13" t="s">
         <v>117</v>
       </c>
-      <c r="O4" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="P4" s="13" t="s">
-        <v>118</v>
-      </c>
       <c r="Q4" s="1" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="R4" s="12" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="S4" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="T4" s="53"/>
     </row>

</xml_diff>